<commit_message>
rill-analysis: After 0.1.0// Add feature: HtmlExporter and JdbcDataRetriever
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/jdbcDataRetriever.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/jdbcDataRetriever.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="2"/>
@@ -13,6 +13,9 @@
     <sheet name="_input2" sheetId="6" r:id="rId4"/>
     <sheet name="_input3" sheetId="7" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="trendChartDataSource" localSheetId="2">OFFSET(_input!$C11,0,0,COUNTA(_input!$A:$A)-1, 4)</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -52,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -150,30 +153,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>db-crm-pss01.db01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yf-crm-pss00.yf01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yf-crm-pss01.yf01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT hostname as '机器名', count(*) as '今日访问量' from crm_tomcat_pangu where ts &gt; DATE_FORMAT(DATE_ADD(NOW(),INTERVAL -2 DAY), '%Y-%m-%d 00:00:00') and ts &lt; DATE_FORMAT(DATE_FORMAT(DATE_ADD(NOW(),INTERVAL -1 DAY), '%Y-%m-%d 00:00:00') group by hostname;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>今日访问量</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SELECT hostname as '机器名', count(*) as '今日访问量' from crm_tomcat_pangu where ts &gt; DATE_FORMAT(DATE_ADD(NOW(),INTERVAL -8 DAY), '%Y-%m-%d 00:00:00') and ts &lt; DATE_FORMAT(DATE_FORMAT(DATE_ADD(NOW(),INTERVAL -7 DAY), '%Y-%m-%d 00:00:00') group by hostname;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>今日访问量</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -194,10 +177,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>当天占比</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>今日总</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -247,13 +226,21 @@
   </si>
   <si>
     <t>SELECT hostname, count(*) from crm_tomcat_pangu where ts &gt; DATEADD('DAY', -1, NOW()) and ts &lt; NOW() group by hostname;</t>
+  </si>
+  <si>
+    <t>SELECT hostname, count(*) from crm_tomcat_pangu where ts &gt; DATEADD('DAY', -2, NOW()) and ts &lt; DATEADD('DAY', -1, NOW()) group by hostname;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT hostname, count(*) from crm_tomcat_pangu where ts &gt; DATEADD('DAY', -8, NOW()) and ts &lt; DATEADD('DAY', -7, NOW()) group by hostname;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,14 +308,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="3" tint="0.39994506668294322"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -368,7 +347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -477,59 +456,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="3" tint="0.79998168889431442"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="3" tint="0.79998168889431442"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.14993743705557422"/>
-      </right>
-      <top style="thin">
-        <color theme="3" tint="0.79998168889431442"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14990691854609822"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="3" tint="0.79998168889431442"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.1498764000366222"/>
-      </right>
-      <top style="thin">
-        <color theme="3" tint="0.79998168889431442"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0" tint="-0.14996795556505021"/>
       </left>
@@ -699,13 +625,65 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="0.79998168889431442"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3" tint="0.79998168889431442"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.1498764000366222"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="0.79998168889431442"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.1498764000366222"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -757,22 +735,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -787,71 +765,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1052,175 +1021,57 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>_input!$D$14</c:f>
+              <c:f>_input!$C$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>今日访问量</c:v>
+                  <c:v>db-crm-pss00.db01</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>_input!$C$15:$C$18</c:f>
+              <c:f>_input!$D$11:$F$11</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>db-crm-pss00.db01</c:v>
+                  <c:v>今日访问量</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>db-crm-pss01.db01</c:v>
+                  <c:v>昨日访问量</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>yf-crm-pss00.yf01</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>yf-crm-pss01.yf01</c:v>
+                  <c:v>上周同期访问量</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>_input!$D$15:$D$18</c:f>
+              <c:f>_input!$D$12:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>47952</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58035</c:v>
+                  <c:v>45583</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48398</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>47624</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>_input!$E$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>昨日访问量</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>_input!$C$15:$C$18</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>db-crm-pss00.db01</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>db-crm-pss01.db01</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>yf-crm-pss00.yf01</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>yf-crm-pss01.yf01</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>_input!$E$15:$E$18</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>45583</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>44037</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45096</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45355</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>_input!$F$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>上周同期访问量</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>_input!$C$15:$C$18</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>db-crm-pss00.db01</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>db-crm-pss01.db01</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>yf-crm-pss00.yf01</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>yf-crm-pss01.yf01</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>_input!$F$15:$F$18</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
                   <c:v>136</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="81740928"/>
-        <c:axId val="81742464"/>
+        <c:axId val="55117696"/>
+        <c:axId val="55119232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81740928"/>
+        <c:axId val="55117696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1229,14 +1080,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81742464"/>
+        <c:crossAx val="55119232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81742464"/>
+        <c:axId val="55119232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1245,13 +1096,14 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81740928"/>
+        <c:crossAx val="55117696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1262,7 +1114,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000966" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000966" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.7500000000000101" l="0.70000000000000062" r="0.70000000000000062" t="0.7500000000000101" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1606,7 +1458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA31"/>
+  <dimension ref="A1:AA28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -1633,7 +1485,7 @@
     </row>
     <row r="2" spans="2:17">
       <c r="B2" s="28" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
@@ -1648,11 +1500,11 @@
       <c r="Q3" s="5"/>
     </row>
     <row r="4" spans="2:17">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
       <c r="Q4" s="5"/>
     </row>
     <row r="5" spans="2:17" ht="3" customHeight="1">
@@ -1714,7 +1566,7 @@
     </row>
     <row r="24" spans="1:27">
       <c r="B24" s="28" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C24" s="28"/>
       <c r="D24" s="28"/>
@@ -1758,65 +1610,65 @@
       <c r="AA26" s="16"/>
     </row>
     <row r="27" spans="1:27" ht="35.25" customHeight="1">
-      <c r="B27" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="47" t="s">
+      <c r="B27" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="35" t="s">
         <v>13</v>
       </c>
       <c r="I27" s="36"/>
       <c r="J27" s="36"/>
       <c r="K27" s="36"/>
       <c r="L27" s="36"/>
-      <c r="M27" s="48"/>
-      <c r="N27" s="41" t="s">
+      <c r="M27" s="40"/>
+      <c r="N27" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="O27" s="42"/>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="42"/>
-      <c r="S27" s="42"/>
-      <c r="T27" s="43"/>
-      <c r="U27" s="35" t="s">
+      <c r="O27" s="31"/>
+      <c r="P27" s="31"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="31"/>
+      <c r="S27" s="31"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="V27" s="36"/>
-      <c r="W27" s="36"/>
-      <c r="X27" s="36"/>
-      <c r="Y27" s="36"/>
-      <c r="Z27" s="36"/>
-      <c r="AA27" s="37"/>
+      <c r="V27" s="31"/>
+      <c r="W27" s="31"/>
+      <c r="X27" s="31"/>
+      <c r="Y27" s="31"/>
+      <c r="Z27" s="31"/>
+      <c r="AA27" s="32"/>
     </row>
     <row r="28" spans="1:27" ht="16.5" customHeight="1">
       <c r="A28" s="22" t="s">
         <v>18</v>
       </c>
       <c r="B28" s="21"/>
-      <c r="C28" s="45" t="str">
-        <f>_input!$C15</f>
+      <c r="C28" s="41" t="str">
+        <f>_input!$C12</f>
         <v>db-crm-pss00.db01</v>
       </c>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="39">
-        <f>_input!$D15</f>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="38">
+        <f>_input!$D12</f>
         <v>47952</v>
       </c>
-      <c r="I28" s="40"/>
-      <c r="J28" s="40"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="40"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
       <c r="M28" s="19"/>
-      <c r="N28" s="38">
-        <f>_input!$J15</f>
+      <c r="N28" s="45">
+        <f>_input!$J12</f>
         <v>2369</v>
       </c>
       <c r="O28" s="34"/>
@@ -1825,18 +1677,18 @@
         <v>16</v>
       </c>
       <c r="R28" s="18">
-        <f>_input!$G15</f>
+        <f>_input!$G12</f>
         <v>5.1971129587784937E-2</v>
       </c>
       <c r="S28" s="18" t="s">
         <v>17</v>
       </c>
       <c r="T28" s="27">
-        <f>_input!$J15</f>
+        <f>_input!$J12</f>
         <v>2369</v>
       </c>
       <c r="U28" s="33">
-        <f>_input!$K15</f>
+        <f>_input!$K12</f>
         <v>47816</v>
       </c>
       <c r="V28" s="34"/>
@@ -1845,235 +1697,34 @@
         <v>16</v>
       </c>
       <c r="Y28" s="18">
-        <f>_input!$H15</f>
+        <f>_input!$H12</f>
         <v>351.58823529411762</v>
       </c>
       <c r="Z28" s="18" t="s">
         <v>17</v>
       </c>
       <c r="AA28" s="20">
-        <f>_input!$K15</f>
+        <f>_input!$K12</f>
         <v>47816</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A29" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="45" t="str">
-        <f>_input!$C16</f>
-        <v>db-crm-pss01.db01</v>
-      </c>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="39">
-        <f>_input!$D16</f>
-        <v>58035</v>
-      </c>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="38">
-        <f>_input!$J16</f>
-        <v>13998</v>
-      </c>
-      <c r="O29" s="34"/>
-      <c r="P29" s="34"/>
-      <c r="Q29" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="R29" s="18">
-        <f>_input!$G16</f>
-        <v>0.3178690646501805</v>
-      </c>
-      <c r="S29" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="T29" s="27">
-        <f>_input!$J16</f>
-        <v>13998</v>
-      </c>
-      <c r="U29" s="33">
-        <f>_input!$K16</f>
-        <v>58022</v>
-      </c>
-      <c r="V29" s="34"/>
-      <c r="W29" s="34"/>
-      <c r="X29" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y29" s="18">
-        <f>_input!$H16</f>
-        <v>4463.2307692307695</v>
-      </c>
-      <c r="Z29" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA29" s="20">
-        <f>_input!$K16</f>
-        <v>58022</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A30" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="45" t="str">
-        <f>_input!$C17</f>
-        <v>yf-crm-pss00.yf01</v>
-      </c>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="39">
-        <f>_input!$D17</f>
-        <v>48398</v>
-      </c>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="40"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="38">
-        <f>_input!$J17</f>
-        <v>3302</v>
-      </c>
-      <c r="O30" s="34"/>
-      <c r="P30" s="34"/>
-      <c r="Q30" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="R30" s="18">
-        <f>_input!$G17</f>
-        <v>7.3221571758027348E-2</v>
-      </c>
-      <c r="S30" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="T30" s="27">
-        <f>_input!$J17</f>
-        <v>3302</v>
-      </c>
-      <c r="U30" s="33">
-        <f>_input!$K17</f>
-        <v>48357</v>
-      </c>
-      <c r="V30" s="34"/>
-      <c r="W30" s="34"/>
-      <c r="X30" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y30" s="18">
-        <f>_input!$H17</f>
-        <v>1179.439024390244</v>
-      </c>
-      <c r="Z30" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA30" s="20">
-        <f>_input!$K17</f>
-        <v>48357</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A31" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="45" t="str">
-        <f>_input!$C18</f>
-        <v>yf-crm-pss01.yf01</v>
-      </c>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="39">
-        <f>_input!$D18</f>
-        <v>47624</v>
-      </c>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="38">
-        <f>_input!$J18</f>
-        <v>2269</v>
-      </c>
-      <c r="O31" s="34"/>
-      <c r="P31" s="34"/>
-      <c r="Q31" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="R31" s="18">
-        <f>_input!$G18</f>
-        <v>5.0027560357182255E-2</v>
-      </c>
-      <c r="S31" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="T31" s="27">
-        <f>_input!$J18</f>
-        <v>2269</v>
-      </c>
-      <c r="U31" s="33">
-        <f>_input!$K18</f>
-        <v>47577</v>
-      </c>
-      <c r="V31" s="34"/>
-      <c r="W31" s="34"/>
-      <c r="X31" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y31" s="18">
-        <f>_input!$H18</f>
-        <v>1012.2765957446809</v>
-      </c>
-      <c r="Z31" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA31" s="20">
-        <f>_input!$K18</f>
-        <v>47577</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="N31:P31"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="U30:W30"/>
-    <mergeCell ref="U31:W31"/>
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="C30:G30"/>
+  <mergeCells count="11">
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="U27:AA27"/>
+    <mergeCell ref="U28:W28"/>
     <mergeCell ref="B27:G27"/>
-    <mergeCell ref="U28:W28"/>
-    <mergeCell ref="U29:W29"/>
-    <mergeCell ref="U27:AA27"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="N27:T27"/>
     <mergeCell ref="N28:P28"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="N27:T27"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:L28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="AA28:AA31">
-    <cfRule type="iconSet" priority="6">
+  <conditionalFormatting sqref="AA28">
+    <cfRule type="iconSet" priority="8">
       <iconSet iconSet="3Arrows" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
@@ -2081,8 +1732,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T28:T31">
-    <cfRule type="iconSet" priority="7">
+  <conditionalFormatting sqref="T28">
+    <cfRule type="iconSet" priority="9">
       <iconSet iconSet="3Arrows" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
@@ -2120,7 +1771,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2128,7 +1779,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2136,7 +1787,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2203,7 +1854,7 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2223,7 +1874,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18" customHeight="1">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="14.25" thickBot="1">
@@ -2242,230 +1893,289 @@
         <v>47952</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="14.25" thickBot="1">
-      <c r="A4" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="3">
-        <v>58035</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="14.25" thickBot="1">
-      <c r="A5" s="23" t="s">
+    <row r="11" spans="1:14">
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="3">
-        <v>48398</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="14.25" thickBot="1">
-      <c r="A6" s="23" t="s">
+      <c r="E11" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="3">
-        <v>47624</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" t="s">
         <v>30</v>
       </c>
-      <c r="E14" t="s">
+      <c r="M11" t="s">
         <v>31</v>
       </c>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="N11" t="s">
         <v>32</v>
       </c>
-      <c r="I14" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14" t="s">
-        <v>43</v>
-      </c>
-      <c r="K14" t="s">
-        <v>44</v>
-      </c>
-      <c r="L14" t="s">
-        <v>36</v>
-      </c>
-      <c r="M14" t="s">
-        <v>37</v>
-      </c>
-      <c r="N14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="C15" s="26" t="str">
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12" s="26" t="str">
         <f>$A3</f>
         <v>db-crm-pss00.db01</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D12" s="24">
         <f>$B3</f>
         <v>47952</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E12" s="24">
         <f>_input2!$B3</f>
         <v>45583</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F12" s="24">
         <f>_input3!$B3</f>
         <v>136</v>
       </c>
+      <c r="G12">
+        <f>IF($E12=0,0,$D12/$E12-1)</f>
+        <v>5.1971129587784937E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ref="H12:H23" si="0">IF($F12=0,0,$D12/$F12-1)</f>
+        <v>351.58823529411762</v>
+      </c>
+      <c r="J12" s="24">
+        <f>$D12-$E12</f>
+        <v>2369</v>
+      </c>
+      <c r="K12" s="24">
+        <f>$D12-$F12</f>
+        <v>47816</v>
+      </c>
+      <c r="L12">
+        <f>SUMIF($D12:$D197,"&gt;0")</f>
+        <v>47952</v>
+      </c>
+      <c r="M12">
+        <f>SUMIF($E12:$E197,"&gt;0")</f>
+        <v>45583</v>
+      </c>
+      <c r="N12">
+        <f>SUMIF($F12:$F197,"&gt;0")</f>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13" s="26">
+        <f t="shared" ref="C13:C23" si="1">$A4</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="24">
+        <f t="shared" ref="D13:D23" si="2">$B4</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="24">
+        <f>_input2!$B4</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="24">
+        <f>_input3!$B4</f>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13:G23" si="3">IF($E13=0,0,$D13/$E13-1)</f>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="24">
+        <f t="shared" ref="J13:J23" si="4">$D13-$E13</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="24">
+        <f t="shared" ref="K13:K23" si="5">$D13-$F13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="C14" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="24">
+        <f>_input2!$B5</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="24">
+        <f>_input3!$B5</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="C15" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="24">
+        <f>_input2!$B6</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="24">
+        <f>_input3!$B6</f>
+        <v>0</v>
+      </c>
       <c r="G15">
-        <f>IF($E15=0,0,$D15/$E15-1)</f>
-        <v>5.1971129587784937E-2</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:H24" si="0">IF($F15=0,0,$D15/$F15-1)</f>
-        <v>351.58823529411762</v>
-      </c>
-      <c r="I15">
-        <f>$D15/$L15</f>
-        <v>0.23737556247493924</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="J15" s="24">
-        <f>$D15-$E15</f>
-        <v>2369</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="K15" s="24">
-        <f>$D15-$F15</f>
-        <v>47816</v>
-      </c>
-      <c r="L15">
-        <f>SUMIF($D15:$D200,"&gt;0")</f>
-        <v>202009</v>
-      </c>
-      <c r="M15">
-        <f>SUMIF($E15:$E200,"&gt;0")</f>
-        <v>180071</v>
-      </c>
-      <c r="N15">
-        <f>SUMIF($F15:$F200,"&gt;0")</f>
-        <v>237</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="C16" s="26" t="str">
-        <f t="shared" ref="C16:C24" si="1">$A4</f>
-        <v>db-crm-pss01.db01</v>
+      <c r="C16" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="D16" s="24">
-        <f t="shared" ref="D16:D24" si="2">$B4</f>
-        <v>58035</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="E16" s="24">
-        <f>_input2!$B4</f>
-        <v>44037</v>
+        <f>_input2!$B7</f>
+        <v>0</v>
       </c>
       <c r="F16" s="24">
-        <f>_input3!$B4</f>
-        <v>13</v>
+        <f>_input3!$B7</f>
+        <v>0</v>
       </c>
       <c r="G16">
-        <f t="shared" ref="G16:G24" si="3">IF($E16=0,0,$D16/$E16-1)</f>
-        <v>0.3178690646501805</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>4463.2307692307695</v>
-      </c>
-      <c r="I16">
-        <f>$D16/$L15</f>
-        <v>0.28728918018504124</v>
+        <v>0</v>
       </c>
       <c r="J16" s="24">
-        <f t="shared" ref="J16:J24" si="4">$D16-$E16</f>
-        <v>13998</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="K16" s="24">
-        <f t="shared" ref="K16:K24" si="5">$D16-$F16</f>
-        <v>58022</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="3:11">
-      <c r="C17" s="26" t="str">
+      <c r="C17" s="26">
         <f t="shared" si="1"/>
-        <v>yf-crm-pss00.yf01</v>
+        <v>0</v>
       </c>
       <c r="D17" s="24">
         <f t="shared" si="2"/>
-        <v>48398</v>
+        <v>0</v>
       </c>
       <c r="E17" s="24">
-        <f>_input2!$B5</f>
-        <v>45096</v>
+        <f>_input2!$B8</f>
+        <v>0</v>
       </c>
       <c r="F17" s="24">
-        <f>_input3!$B5</f>
-        <v>41</v>
+        <f>_input3!$B8</f>
+        <v>0</v>
       </c>
       <c r="G17">
         <f t="shared" si="3"/>
-        <v>7.3221571758027348E-2</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>1179.439024390244</v>
-      </c>
-      <c r="I17">
-        <f>$D17/$L15</f>
-        <v>0.23958338489869263</v>
+        <v>0</v>
       </c>
       <c r="J17" s="24">
         <f t="shared" si="4"/>
-        <v>3302</v>
+        <v>0</v>
       </c>
       <c r="K17" s="24">
         <f t="shared" si="5"/>
-        <v>48357</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="3:11">
-      <c r="C18" s="26" t="str">
+      <c r="C18" s="26">
         <f t="shared" si="1"/>
-        <v>yf-crm-pss01.yf01</v>
+        <v>0</v>
       </c>
       <c r="D18" s="24">
         <f t="shared" si="2"/>
-        <v>47624</v>
+        <v>0</v>
       </c>
       <c r="E18" s="24">
-        <f>_input2!$B6</f>
-        <v>45355</v>
+        <f>_input2!$B9</f>
+        <v>0</v>
       </c>
       <c r="F18" s="24">
-        <f>_input3!$B6</f>
-        <v>47</v>
+        <f>_input3!$B9</f>
+        <v>0</v>
       </c>
       <c r="G18">
         <f t="shared" si="3"/>
-        <v>5.0027560357182255E-2</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>1012.2765957446809</v>
-      </c>
-      <c r="I18">
-        <f>$D18/$L15</f>
-        <v>0.23575187244132687</v>
+        <v>0</v>
       </c>
       <c r="J18" s="24">
         <f t="shared" si="4"/>
-        <v>2269</v>
+        <v>0</v>
       </c>
       <c r="K18" s="24">
         <f t="shared" si="5"/>
-        <v>47577</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="3:11">
@@ -2478,11 +2188,11 @@
         <v>0</v>
       </c>
       <c r="E19" s="24">
-        <f>_input2!$B7</f>
+        <f>_input2!$B10</f>
         <v>0</v>
       </c>
       <c r="F19" s="24">
-        <f>_input3!$B7</f>
+        <f>_input3!$B10</f>
         <v>0</v>
       </c>
       <c r="G19">
@@ -2491,10 +2201,6 @@
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <f>$D19/$L15</f>
         <v>0</v>
       </c>
       <c r="J19" s="24">
@@ -2516,11 +2222,11 @@
         <v>0</v>
       </c>
       <c r="E20" s="24">
-        <f>_input2!$B8</f>
+        <f>_input2!$B11</f>
         <v>0</v>
       </c>
       <c r="F20" s="24">
-        <f>_input3!$B8</f>
+        <f>_input3!$B11</f>
         <v>0</v>
       </c>
       <c r="G20">
@@ -2529,10 +2235,6 @@
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f>$D20/$L15</f>
         <v>0</v>
       </c>
       <c r="J20" s="24">
@@ -2554,11 +2256,11 @@
         <v>0</v>
       </c>
       <c r="E21" s="24">
-        <f>_input2!$B9</f>
+        <f>_input2!$B12</f>
         <v>0</v>
       </c>
       <c r="F21" s="24">
-        <f>_input3!$B9</f>
+        <f>_input3!$B12</f>
         <v>0</v>
       </c>
       <c r="G21">
@@ -2567,10 +2269,6 @@
       </c>
       <c r="H21">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <f>$D21/$L15</f>
         <v>0</v>
       </c>
       <c r="J21" s="24">
@@ -2588,15 +2286,15 @@
         <v>0</v>
       </c>
       <c r="D22" s="24">
-        <f>$B10</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E22" s="24">
-        <f>_input2!$B10</f>
+        <f>_input2!$B13</f>
         <v>0</v>
       </c>
       <c r="F22" s="24">
-        <f>_input3!$B10</f>
+        <f>_input3!$B13</f>
         <v>0</v>
       </c>
       <c r="G22">
@@ -2605,10 +2303,6 @@
       </c>
       <c r="H22">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <f>$D22/$L15</f>
         <v>0</v>
       </c>
       <c r="J22" s="24">
@@ -2626,15 +2320,15 @@
         <v>0</v>
       </c>
       <c r="D23" s="24">
-        <f>$B11</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E23" s="24">
-        <f>_input2!$B11</f>
+        <f>_input2!$B14</f>
         <v>0</v>
       </c>
       <c r="F23" s="24">
-        <f>_input3!$B11</f>
+        <f>_input3!$B14</f>
         <v>0</v>
       </c>
       <c r="G23">
@@ -2645,10 +2339,6 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I23">
-        <f>$D23/$L15</f>
-        <v>0</v>
-      </c>
       <c r="J23" s="24">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2659,51 +2349,7 @@
       </c>
     </row>
     <row r="24" spans="3:11">
-      <c r="C24" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D24" s="24">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="24">
-        <f>_input2!$B12</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="24">
-        <f>_input3!$B12</f>
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <f>$D24/$L15</f>
-        <v>0</v>
-      </c>
-      <c r="J24" s="24">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="24">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="3:11">
-      <c r="C25" s="25"/>
-    </row>
-    <row r="26" spans="3:11">
-      <c r="C26" s="25"/>
-    </row>
-    <row r="27" spans="3:11">
-      <c r="C27" s="25"/>
+      <c r="C24" s="25"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2717,10 +2363,60 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="13.75" customWidth="1"/>
+    <col min="5" max="5" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" customHeight="1">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25" thickBot="1">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.25" thickBot="1">
+      <c r="A3" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45583</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.25" customHeight="1"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2737,7 +2433,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25" thickBot="1">
@@ -2745,7 +2441,7 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" thickBot="1">
@@ -2753,106 +2449,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="3">
-        <v>45583</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A4" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="3">
-        <v>44037</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A5" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="3">
-        <v>45096</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A6" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="3">
-        <v>45355</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <tabColor rgb="FF7030A0"/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="20.625" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="13.75" customWidth="1"/>
-    <col min="5" max="5" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.25" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="18" customHeight="1">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A3" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="3">
         <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A4" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A5" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="3">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A6" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="3">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>